<commit_message>
upload file error fixed
</commit_message>
<xml_diff>
--- a/BlockChain_code_File-main/public/excel/data.xlsx
+++ b/BlockChain_code_File-main/public/excel/data.xlsx
@@ -10,7 +10,7 @@
     <sheet name="June Ui" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'June Ui'!$A$1:$H$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'June Ui'!$A$1:$H$3</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>S/No</t>
   </si>
@@ -72,19 +72,10 @@
     <t>Certificate_Name</t>
   </si>
   <si>
-    <t>Minor Test.pdf</t>
+    <t>HR_Oyester.pdf</t>
   </si>
   <si>
-    <t>minor_fluid_1916083 (1).pdf</t>
-  </si>
-  <si>
-    <t>Web dev</t>
-  </si>
-  <si>
-    <t>pdf.pdf</t>
-  </si>
-  <si>
-    <t>Employee 3</t>
+    <t>rv.pdf</t>
   </si>
 </sst>
 </file>
@@ -154,7 +145,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -177,19 +168,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="22"/>
-      </left>
-      <right style="thin">
-        <color indexed="22"/>
-      </right>
-      <top style="thin">
-        <color indexed="22"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -197,7 +175,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -239,19 +217,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="15" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
@@ -260,6 +225,16 @@
     <cellStyle name="Normal_TRUE_2" xfId="2"/>
   </cellStyles>
   <dxfs count="11">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -415,16 +390,6 @@
       </fill>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -439,19 +404,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J4" totalsRowShown="0" headerRowDxfId="9">
-  <autoFilter ref="A1:J4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J3" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="A1:J3"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="S/No" dataDxfId="8"/>
-    <tableColumn id="2" name="Batch Code" dataDxfId="7" dataCellStyle="Normal_TRUE"/>
+    <tableColumn id="1" name="S/No" dataDxfId="9"/>
+    <tableColumn id="2" name="Batch Code" dataDxfId="8" dataCellStyle="Normal_TRUE"/>
     <tableColumn id="3" name="Staff_Name"/>
-    <tableColumn id="4" name="Staff_EmpNumber" dataDxfId="6"/>
-    <tableColumn id="5" name="TrainingTitle" dataDxfId="5"/>
-    <tableColumn id="6" name="TrainingCode" dataDxfId="4"/>
-    <tableColumn id="7" name="Batch_Trainer" dataDxfId="3"/>
-    <tableColumn id="8" name="BatchStartDate" dataDxfId="2" dataCellStyle="Normal_TRUE"/>
-    <tableColumn id="9" name="Staff_Email" dataDxfId="1" dataCellStyle="Hyperlink"/>
-    <tableColumn id="10" name="Certificate_Name" dataDxfId="0"/>
+    <tableColumn id="4" name="Staff_EmpNumber" dataDxfId="7"/>
+    <tableColumn id="5" name="TrainingTitle" dataDxfId="6"/>
+    <tableColumn id="6" name="TrainingCode" dataDxfId="5"/>
+    <tableColumn id="7" name="Batch_Trainer" dataDxfId="4"/>
+    <tableColumn id="8" name="BatchStartDate" dataDxfId="3" dataCellStyle="Normal_TRUE"/>
+    <tableColumn id="9" name="Staff_Email" dataDxfId="2" dataCellStyle="Hyperlink"/>
+    <tableColumn id="10" name="Certificate_Name" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -712,7 +677,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -720,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J202"/>
+  <dimension ref="A1:J201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -837,36 +802,14 @@
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="17">
-        <v>2</v>
-      </c>
-      <c r="B4" s="18">
-        <v>6940</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="17">
-        <v>3</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="17">
-        <v>12</v>
-      </c>
-      <c r="G4" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" s="14" t="s">
-        <v>19</v>
-      </c>
+      <c r="A4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="10"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="7"/>
@@ -980,11 +923,11 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="7"/>
-      <c r="B16" s="8"/>
+      <c r="B16" s="11"/>
       <c r="C16"/>
       <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
       <c r="G16" s="7"/>
       <c r="H16" s="10"/>
     </row>
@@ -1100,11 +1043,11 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="7"/>
-      <c r="B28" s="11"/>
+      <c r="B28" s="8"/>
       <c r="C28"/>
       <c r="D28" s="7"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
       <c r="G28" s="7"/>
       <c r="H28" s="10"/>
     </row>
@@ -1230,11 +1173,11 @@
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="7"/>
-      <c r="B41" s="8"/>
+      <c r="B41" s="11"/>
       <c r="C41"/>
       <c r="D41" s="7"/>
-      <c r="E41" s="9"/>
-      <c r="F41" s="9"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
       <c r="G41" s="7"/>
       <c r="H41" s="10"/>
     </row>
@@ -1320,11 +1263,11 @@
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="7"/>
-      <c r="B50" s="11"/>
+      <c r="B50" s="8"/>
       <c r="C50"/>
       <c r="D50" s="7"/>
-      <c r="E50" s="12"/>
-      <c r="F50" s="12"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
       <c r="G50" s="7"/>
       <c r="H50" s="10"/>
     </row>
@@ -1600,11 +1543,11 @@
     </row>
     <row r="78" spans="1:8">
       <c r="A78" s="7"/>
-      <c r="B78" s="8"/>
+      <c r="B78" s="7"/>
       <c r="C78"/>
       <c r="D78" s="7"/>
-      <c r="E78" s="9"/>
-      <c r="F78" s="9"/>
+      <c r="E78" s="7"/>
+      <c r="F78" s="7"/>
       <c r="G78" s="7"/>
       <c r="H78" s="10"/>
     </row>
@@ -1839,14 +1782,7 @@
       <c r="H101" s="10"/>
     </row>
     <row r="102" spans="1:8">
-      <c r="A102" s="7"/>
-      <c r="B102" s="7"/>
-      <c r="C102"/>
-      <c r="D102" s="7"/>
-      <c r="E102" s="7"/>
-      <c r="F102" s="7"/>
       <c r="G102" s="7"/>
-      <c r="H102" s="10"/>
     </row>
     <row r="103" spans="1:8">
       <c r="G103" s="7"/>
@@ -1888,7 +1824,7 @@
       <c r="G115" s="7"/>
     </row>
     <row r="116" spans="7:7">
-      <c r="G116" s="7"/>
+      <c r="G116" s="12"/>
     </row>
     <row r="117" spans="7:7">
       <c r="G117" s="12"/>
@@ -1924,7 +1860,7 @@
       <c r="G127" s="12"/>
     </row>
     <row r="128" spans="7:7">
-      <c r="G128" s="12"/>
+      <c r="G128" s="9"/>
     </row>
     <row r="129" spans="7:7">
       <c r="G129" s="9"/>
@@ -1963,7 +1899,7 @@
       <c r="G140" s="9"/>
     </row>
     <row r="141" spans="7:7">
-      <c r="G141" s="9"/>
+      <c r="G141" s="12"/>
     </row>
     <row r="142" spans="7:7">
       <c r="G142" s="12"/>
@@ -1990,7 +1926,7 @@
       <c r="G149" s="12"/>
     </row>
     <row r="150" spans="7:7">
-      <c r="G150" s="12"/>
+      <c r="G150" s="9"/>
     </row>
     <row r="151" spans="7:7">
       <c r="G151" s="9"/>
@@ -2074,7 +2010,7 @@
       <c r="G177" s="9"/>
     </row>
     <row r="178" spans="7:7">
-      <c r="G178" s="9"/>
+      <c r="G178" s="7"/>
     </row>
     <row r="179" spans="7:7">
       <c r="G179" s="7"/>
@@ -2145,12 +2081,9 @@
     <row r="201" spans="7:7">
       <c r="G201" s="7"/>
     </row>
-    <row r="202" spans="7:7">
-      <c r="G202" s="7"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D102">
-    <cfRule type="duplicateValues" dxfId="10" priority="4"/>
+  <conditionalFormatting sqref="D2:D101">
+    <cfRule type="duplicateValues" dxfId="0" priority="5"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1"/>
@@ -2164,61 +2097,61 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<XMLData TextToDisplay="%HOSTNAME%">WCB00094282.etisalat.corp.ae</XMLData>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<XMLData TextToDisplay="%CLASSIFICATIONDATETIME%">10:19 01/09/2019</XMLData>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<XMLData TextToDisplay="RightsWATCHMark">76|Etisalat-Group-Internal|{00000000-0000-0000-0000-000000000000}</XMLData>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <XMLData TextToDisplay="%DOCUMENTGUID%">{00000000-0000-0000-0000-000000000000}</XMLData>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="RightsWATCHMark">76|Etisalat-Group-Internal|{00000000-0000-0000-0000-000000000000}</XMLData>
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<XMLData TextToDisplay="%EMAILADDRESS%">mohammshahin@etisalat.ae</XMLData>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%CLASSIFICATIONDATETIME%">10:19 01/09/2019</XMLData>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%HOSTNAME%">WCB00094282.etisalat.corp.ae</XMLData>
-</file>
-
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
 <XMLData TextToDisplay="%USERNAME%">mohammshahin</XMLData>
 </file>
 
-<file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%EMAILADDRESS%">mohammshahin@etisalat.ae</XMLData>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9FD55538-6D4B-425F-B44D-4015B7E9E399}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97F6B195-C060-43AA-A24A-6190B6CF0D70}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5375092-E49A-46E6-A2BF-AF82C0840F59}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{158E32D4-C0BA-4AEA-B8E7-E2B73F1D51AA}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5375092-E49A-46E6-A2BF-AF82C0840F59}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97F6B195-C060-43AA-A24A-6190B6CF0D70}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9FD55538-6D4B-425F-B44D-4015B7E9E399}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78B9DA3B-989B-4D15-9A99-8576DAF2B73D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF54BAE9-5F59-4D3F-ADAE-3F6AC2F1C876}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF54BAE9-5F59-4D3F-ADAE-3F6AC2F1C876}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78B9DA3B-989B-4D15-9A99-8576DAF2B73D}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
</xml_diff>